<commit_message>
Work on BOSE/detector crosstalk, feedhorn drawing.
</commit_message>
<xml_diff>
--- a/support/1k-heat-loads.xlsx
+++ b/support/1k-heat-loads.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
   <si>
     <t>#</t>
   </si>
@@ -74,6 +74,9 @@
   <si>
     <t>1004 Total</t>
   </si>
+  <si>
+    <t>BOSE inputs</t>
+  </si>
 </sst>
 </file>
 
@@ -81,7 +84,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.000"/>
-    <numFmt numFmtId="166" formatCode="0.0"/>
+    <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -125,7 +128,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
@@ -429,10 +432,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H13"/>
+  <dimension ref="A1:H19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -532,28 +535,41 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4">
+        <v>4</v>
+      </c>
+      <c r="C4" s="1">
+        <f>PI()*(0.005/2)^2*25.4^2</f>
+        <v>1.2667686977437443E-2</v>
+      </c>
+      <c r="D4" s="1">
+        <v>1</v>
+      </c>
+      <c r="E4" s="2">
+        <f>(C4/1000^2)/D4*1000</f>
+        <v>1.2667686977437441E-5</v>
+      </c>
+      <c r="F4">
+        <f>10000/1000</f>
+        <v>10</v>
+      </c>
+      <c r="G4" s="3">
+        <f>B4*E4*F4*1000000</f>
+        <v>506.7074790974977</v>
+      </c>
+      <c r="H4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="1">
+      <c r="B5" s="1">
         <f>8*32</f>
         <v>256</v>
-      </c>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="2">
-        <f>B4*(0.01)^2*(0.00018)*1000000</f>
-        <v>4.6080000000000005</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5" s="1">
-        <f>4*B4</f>
-        <v>1024</v>
       </c>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
@@ -561,85 +577,116 @@
       <c r="F5" s="1"/>
       <c r="G5" s="2">
         <f>B5*(0.01)^2*(0.00018)*1000000</f>
-        <v>18.432000000000002</v>
+        <v>4.6080000000000005</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B6" s="1">
-        <v>251</v>
+        <f>4*B5</f>
+        <v>1024</v>
       </c>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
       <c r="G6" s="2">
-        <f>0.000000001*B6*1000000</f>
-        <v>0.251</v>
+        <f>B6*(0.01)^2*(0.00018)*1000000</f>
+        <v>18.432000000000002</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7">
-        <f>4*B6</f>
-        <v>1004</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="B7" s="1">
+        <v>251</v>
+      </c>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
       <c r="G7" s="2">
         <f>0.000000001*B7*1000000</f>
+        <v>0.251</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8">
+        <f>4*B7</f>
+        <v>1004</v>
+      </c>
+      <c r="G8" s="2">
+        <f>0.000000001*B8*1000000</f>
         <v>1.004</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="5" t="s">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B9">
+      <c r="B10">
         <v>16</v>
       </c>
-      <c r="C9">
+      <c r="C10">
         <f>(0.016*0.1)*(25.4)^2</f>
         <v>1.0322560000000001</v>
       </c>
-      <c r="D9">
+      <c r="D10">
         <f>1.5*25.4/1000</f>
         <v>3.8099999999999995E-2</v>
       </c>
-      <c r="E9" s="2">
-        <f>(C9/1000^2)/D9*1000</f>
+      <c r="E10" s="2">
+        <f>(C10/1000^2)/D10*1000</f>
         <v>2.7093333333333341E-2</v>
       </c>
-      <c r="F9">
+      <c r="F10">
         <f>75*(6.4^2 - 1^2)*0.000001/10</f>
         <v>2.9970000000000007E-4</v>
       </c>
-      <c r="G9" s="3">
-        <f>B9*E9*F9*1000000</f>
+      <c r="G10" s="3">
+        <f>B10*E10*F10*1000000</f>
         <v>129.91795200000004</v>
       </c>
-      <c r="H9" t="s">
+      <c r="H10" t="s">
         <v>14</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="F12" t="s">
-        <v>15</v>
-      </c>
-      <c r="G12" s="2">
-        <f>G2+G4+G6+G9</f>
-        <v>184.31394192526915</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F13" t="s">
+        <v>15</v>
+      </c>
+      <c r="G13" s="2">
+        <f>G2+G5+G7+G10</f>
+        <v>184.31394192526915</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F14" t="s">
         <v>16</v>
       </c>
-      <c r="G13" s="2">
-        <f>G3+G5+G7+G9</f>
+      <c r="G14" s="2">
+        <f>G3+G6+G8+G10</f>
         <v>273.19642681317282</v>
+      </c>
+    </row>
+    <row r="17" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F17">
+        <v>49.9818</v>
+      </c>
+      <c r="G17">
+        <v>0.101481</v>
+      </c>
+    </row>
+    <row r="19" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F19">
+        <f>F17/G17</f>
+        <v>492.52372365270344</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
More ch 4 edits
</commit_message>
<xml_diff>
--- a/support/1k-heat-loads.xlsx
+++ b/support/1k-heat-loads.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="150" windowWidth="18195" windowHeight="7485"/>
+    <workbookView xWindow="360" yWindow="150" windowWidth="15210" windowHeight="7485"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="26">
   <si>
     <t>#</t>
   </si>
@@ -75,7 +75,31 @@
     <t>1004 Total</t>
   </si>
   <si>
-    <t>BOSE inputs</t>
+    <t>BOSE inputs (from 300K)</t>
+  </si>
+  <si>
+    <t>BOSE inputs (from 50K)</t>
+  </si>
+  <si>
+    <t>BOSE inputs (from 4K)</t>
+  </si>
+  <si>
+    <t>Other in-band optical power</t>
+  </si>
+  <si>
+    <t>Series Arrays (251 detectors)</t>
+  </si>
+  <si>
+    <t>Series Arrays (1004 detectors)</t>
+  </si>
+  <si>
+    <t>Mux Chips (251 detectors)</t>
+  </si>
+  <si>
+    <t>Mux Chips (1004 detectors)</t>
+  </si>
+  <si>
+    <t>100 uA Ic, R_dyn = 5 Ohm (see QSP wiki)</t>
   </si>
 </sst>
 </file>
@@ -124,13 +148,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -432,10 +457,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H19"/>
+  <dimension ref="A1:H18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -445,7 +470,7 @@
     <col min="4" max="4" width="6" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="25.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.28515625" customWidth="1"/>
+    <col min="7" max="7" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -482,12 +507,12 @@
         <v>1.2667686977437443E-2</v>
       </c>
       <c r="D2" s="1">
-        <f>0.4</f>
-        <v>0.4</v>
+        <f>1.04 - 2*(13*2.54/100)</f>
+        <v>0.37959999999999994</v>
       </c>
       <c r="E2" s="2">
         <f>(C2/1000^2)/D2*1000</f>
-        <v>3.1669217443593599E-5</v>
+        <v>3.3371145883660284E-5</v>
       </c>
       <c r="F2" s="2">
         <f>(8.8 - 0.11)/1000</f>
@@ -495,7 +520,7 @@
       </c>
       <c r="G2" s="3">
         <f>B2*E2*F2*1000000</f>
-        <v>49.536989925269111</v>
+        <v>52.199146391221433</v>
       </c>
       <c r="H2" t="s">
         <v>5</v>
@@ -514,12 +539,12 @@
         <v>1.2667686977437443E-2</v>
       </c>
       <c r="D3" s="1">
-        <f>0.4</f>
-        <v>0.4</v>
+        <f>1.04 - 2*(13*2.54/100)</f>
+        <v>0.37959999999999994</v>
       </c>
       <c r="E3" s="2">
         <f>(C3/1000^2)/D3*1000</f>
-        <v>3.1669217443593599E-5</v>
+        <v>3.3371145883660284E-5</v>
       </c>
       <c r="F3" s="2">
         <f>(8.8 - 0.11)/1000</f>
@@ -527,7 +552,7 @@
       </c>
       <c r="G3" s="3">
         <f>B3*E3*F3*1000000</f>
-        <v>123.84247481317279</v>
+        <v>130.49786597805357</v>
       </c>
       <c r="H3" t="s">
         <v>5</v>
@@ -552,12 +577,12 @@
         <v>1.2667686977437441E-5</v>
       </c>
       <c r="F4">
-        <f>10000/1000</f>
-        <v>10</v>
+        <f>(10000-0.11)/1000</f>
+        <v>9.9998899999999988</v>
       </c>
       <c r="G4" s="3">
         <f>B4*E4*F4*1000000</f>
-        <v>506.7074790974977</v>
+        <v>506.70190531522752</v>
       </c>
       <c r="H4" t="s">
         <v>5</v>
@@ -565,128 +590,223 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5">
+        <v>4</v>
+      </c>
+      <c r="C5" s="1">
+        <f>PI()*(0.005/2)^2*25.4^2</f>
+        <v>1.2667686977437443E-2</v>
+      </c>
+      <c r="D5" s="1">
+        <v>1</v>
+      </c>
+      <c r="E5" s="2">
+        <f>(C5/1000^2)/D5*1000</f>
+        <v>1.2667686977437441E-5</v>
+      </c>
+      <c r="F5">
+        <f>(1300-0.11)/1000</f>
+        <v>1.29989</v>
+      </c>
+      <c r="G5" s="3">
+        <f>B5*E5*F5*1000000</f>
+        <v>65.866398500404628</v>
+      </c>
+      <c r="H5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6">
+        <v>4</v>
+      </c>
+      <c r="C6" s="1">
+        <f>PI()*(0.005/2)^2*25.4^2</f>
+        <v>1.2667686977437443E-2</v>
+      </c>
+      <c r="D6" s="1">
+        <f>12*2.54/100</f>
+        <v>0.30480000000000002</v>
+      </c>
+      <c r="E6" s="2">
+        <f>(C6/1000^2)/D6*1000</f>
+        <v>4.1560652813114968E-5</v>
+      </c>
+      <c r="F6">
+        <f>(6.5-0.11)/1000</f>
+        <v>6.3899999999999998E-3</v>
+      </c>
+      <c r="G6" s="3">
+        <f>B6*E6*F6*1000000</f>
+        <v>1.0622902859032186</v>
+      </c>
+      <c r="H6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="1">
+      <c r="B7" s="1">
         <f>8*32</f>
         <v>256</v>
-      </c>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-      <c r="G5" s="2">
-        <f>B5*(0.01)^2*(0.00018)*1000000</f>
-        <v>4.6080000000000005</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" s="1">
-        <f>4*B5</f>
-        <v>1024</v>
-      </c>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
-      <c r="G6" s="2">
-        <f>B6*(0.01)^2*(0.00018)*1000000</f>
-        <v>18.432000000000002</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B7" s="1">
-        <v>251</v>
       </c>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
-      <c r="G7" s="2">
-        <f>0.000000001*B7*1000000</f>
-        <v>0.251</v>
+      <c r="G7" s="3">
+        <f>B7*(0.01)^2*(0.00018)*1000000</f>
+        <v>4.6080000000000005</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" s="1">
+        <f>4*B7</f>
+        <v>1024</v>
+      </c>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="3">
+        <f>B8*(0.01)^2*(0.00018)*1000000</f>
+        <v>18.432000000000002</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" s="1">
+        <v>251</v>
+      </c>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="3">
+        <f>0.000000001*B9*1000000</f>
+        <v>0.251</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B8">
-        <f>4*B7</f>
+      <c r="B10">
+        <f>4*B9</f>
         <v>1004</v>
       </c>
-      <c r="G8" s="2">
-        <f>0.000000001*B8*1000000</f>
+      <c r="G10" s="3">
+        <f>0.000000001*B10*1000000</f>
         <v>1.004</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="5" t="s">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B10">
+      <c r="B11">
         <v>16</v>
       </c>
-      <c r="C10">
+      <c r="C11">
         <f>(0.016*0.1)*(25.4)^2</f>
         <v>1.0322560000000001</v>
       </c>
-      <c r="D10">
+      <c r="D11">
         <f>1.5*25.4/1000</f>
         <v>3.8099999999999995E-2</v>
       </c>
-      <c r="E10" s="2">
-        <f>(C10/1000^2)/D10*1000</f>
+      <c r="E11" s="2">
+        <f>(C11/1000^2)/D11*1000</f>
         <v>2.7093333333333341E-2</v>
       </c>
-      <c r="F10">
-        <f>75*(6.4^2 - 1^2)*0.000001/10</f>
-        <v>2.9970000000000007E-4</v>
-      </c>
-      <c r="G10" s="3">
-        <f>B10*E10*F10*1000000</f>
-        <v>129.91795200000004</v>
-      </c>
-      <c r="H10" t="s">
+      <c r="F11">
+        <f>170/2.1*(6.4^2.1 - 1^2.1)*0.000001/10</f>
+        <v>3.9112042468723401E-4</v>
+      </c>
+      <c r="G11" s="3">
+        <f>B11*E11*F11*1000000</f>
+        <v>169.54809663241807</v>
+      </c>
+      <c r="H11" t="s">
         <v>14</v>
       </c>
     </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E12" s="2"/>
+      <c r="G12" s="3">
+        <v>5.6</v>
+      </c>
+    </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="F13" t="s">
+      <c r="A13" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="G13" s="6">
+        <f>0.02*8</f>
+        <v>0.16</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="G14" s="6">
+        <f>0.02*32</f>
+        <v>0.64</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="G15" s="6">
+        <f>8*5*(0.0001)^2*1000000</f>
+        <v>0.39999999999999997</v>
+      </c>
+      <c r="H15" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="G16" s="6">
+        <f>32*5*(0.0001)^2*1000000</f>
+        <v>1.5999999999999999</v>
+      </c>
+    </row>
+    <row r="17" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F17" t="s">
         <v>15</v>
       </c>
-      <c r="G13" s="2">
-        <f>G2+G5+G7+G10</f>
-        <v>184.31394192526915</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="F14" t="s">
+      <c r="G17" s="3">
+        <f>G2+G7+G9+G11+G4+G12+G13+G15</f>
+        <v>739.46814833886697</v>
+      </c>
+    </row>
+    <row r="18" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F18" t="s">
         <v>16</v>
       </c>
-      <c r="G14" s="2">
-        <f>G3+G6+G8+G10</f>
-        <v>273.19642681317282</v>
-      </c>
-    </row>
-    <row r="17" spans="6:7" x14ac:dyDescent="0.25">
-      <c r="F17">
-        <v>49.9818</v>
-      </c>
-      <c r="G17">
-        <v>0.101481</v>
-      </c>
-    </row>
-    <row r="19" spans="6:7" x14ac:dyDescent="0.25">
-      <c r="F19">
-        <f>F17/G17</f>
-        <v>492.52372365270344</v>
+      <c r="G18" s="3">
+        <f>G3+G8+G10+G11+G4+G12+G14+G16</f>
+        <v>834.02386792569916</v>
       </c>
     </row>
   </sheetData>

</xml_diff>